<commit_message>
Circulars and Regulations prompt added
</commit_message>
<xml_diff>
--- a/data/output_excels/2025-12-08_to_2025-12-14/AIF.xlsx
+++ b/data/output_excels/2025-12-08_to_2025-12-14/AIF.xlsx
@@ -524,12 +524,12 @@
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>• The amendment expands the definition of promoter(s) in Real Estate Investment Trusts (REITs), including those with the same promoters, even if they are not directly involved.
-• It eliminates certain sub-clauses related to company or LLP group companies and entities under the same management.
-• The amendment clarifies that common infrastructure can include facilities like power plants, water treatment plants, etc., regardless of location within a project.
-• Excess production from common infrastructure can now be sold or supplied to grids or utilities, subject to regulations.
-• The amendment defines debt securities according to the SEBI (Issue and Listing of Debt Securities) Regulations, 2008.
-• It introduces an employee unit option scheme where the manager can grant unit options to its employees through an employee benefit trust. Employees include all directors except independent directors.</t>
+          <t>• The amendment introduces changes to the definition of "controlling interest" for Real Estate Investment Trusts (REITs), depending on whether their shares are listed or not.
+• If listed, the definition will align with regulations under Section 11 of the SEBI Act and the Companies Act, 2013. If unlisted, it will follow the Companies Act, 2013 definition.
+• The amendment expands the definition of "common infrastructure" to include facilities such as power plants, water treatment plants, waste treatment plants, and other amenities that exclusively supply or cater to REIT, its HoldCo(s) or SPV(s).
+• Any excess production or capacity from common infrastructure can now be sold or supplied to a central or state grid or utility, subject to specific conditions.
+• The amendment adds a new definition for "employee unit option scheme," which is a scheme under which the manager grants unit options to its employees through an employee benefit trust.
+• Employees of the manager will include all directors, except independent directors.</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">

</xml_diff>